<commit_message>
Fixed bugs and Exam DEC added
</commit_message>
<xml_diff>
--- a/TE A TT.xlsx
+++ b/TE A TT.xlsx
@@ -1,64 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Project\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE048E0-7D10-4AFA-A4EC-3A6FEB871629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9960"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Table 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Table 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Table 2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="66">
-  <si>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-      </rPr>
-      <t xml:space="preserve">Mahatma Education Society's
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-      </rPr>
-      <t xml:space="preserve">Pillai HOC College of Engineering and Technology Department of Computer Engineering
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-      </rPr>
-      <t xml:space="preserve">w.e.f 4th September 2023 OSAY 2023-2024
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-      </rPr>
-      <t>TE COMP A</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <r>
       <rPr>
@@ -1442,68 +1404,14 @@
         <rFont val="Tahoma"/>
       </rPr>
       <t>Shrutika Khobragade, Srijita Bhattacharjee</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <rFont val="Tahoma"/>
-      </rPr>
-      <t>Ms.Pradnya Patil</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <rFont val="Tahoma"/>
-      </rPr>
-      <t>Ms. Rohini Bhosale</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <rFont val="Tahoma"/>
-      </rPr>
-      <t>Dr.J.W.Bakal</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <rFont val="Tahoma"/>
-      </rPr>
-      <t>Timetable Co-ordinator</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <rFont val="Tahoma"/>
-      </rPr>
-      <t>HoD</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <rFont val="Tahoma"/>
-      </rPr>
-      <t>Principal</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1523,20 +1431,6 @@
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1564,7 +1458,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1694,21 +1588,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="26">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1744,9 +1629,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1759,6 +1641,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1776,57 +1670,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2129,470 +1972,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.77734375" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" customWidth="1"/>
-    <col min="4" max="8" width="8.6640625" customWidth="1"/>
-    <col min="9" max="9" width="2.109375" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" customWidth="1"/>
-    <col min="11" max="11" width="3" customWidth="1"/>
-    <col min="13" max="13" width="0.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" ht="108" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-    </row>
-    <row r="2" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="S2" s="29"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="V2" s="29"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="S3" s="29"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="V3" s="29"/>
-      <c r="W3" s="30"/>
-      <c r="X3" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="32"/>
-      <c r="N4" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="S4" s="29"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="V4" s="29"/>
-      <c r="W4" s="30"/>
-      <c r="X4" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="S5" s="29"/>
-      <c r="T5" s="30"/>
-      <c r="U5" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="V5" s="29"/>
-      <c r="W5" s="30"/>
-      <c r="X5" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="36"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="36"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="30"/>
-      <c r="X6" s="8"/>
-    </row>
-    <row r="7" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="S7" s="29"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="V7" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="W7" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="X7" s="9"/>
-    </row>
-    <row r="8" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="S8" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="T8" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="U8" s="38"/>
-      <c r="V8" s="38"/>
-      <c r="W8" s="38"/>
-      <c r="X8" s="9"/>
-    </row>
-    <row r="9" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I9" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="J9" s="30"/>
-      <c r="K9" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" s="30"/>
-      <c r="M9" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="N9" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="O9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="P9" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q9" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="R9" s="38"/>
-      <c r="S9" s="38"/>
-      <c r="T9" s="38"/>
-      <c r="U9" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="V9" s="29"/>
-      <c r="W9" s="30"/>
-      <c r="X9" s="9"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X100"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
@@ -2621,328 +2004,328 @@
   <sheetData>
     <row r="1" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="22" t="s">
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="17" t="s">
+      <c r="S1" s="13"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="14"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="17" t="s">
+      <c r="V1" s="13"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="V1" s="14"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="18" t="s">
+      <c r="E2" s="22"/>
+      <c r="F2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="22"/>
+      <c r="H2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="13" t="s">
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="13" t="s">
+      <c r="S2" s="13"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="14"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="13" t="s">
+      <c r="V2" s="13"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="V2" s="14"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="18" t="s">
+      <c r="I3" s="22"/>
+      <c r="J3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="18" t="s">
+      <c r="K3" s="22"/>
+      <c r="L3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="19"/>
-      <c r="L3" s="18" t="s">
+      <c r="M3" s="22"/>
+      <c r="N3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="19"/>
-      <c r="N3" s="13" t="s">
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="13" t="s">
+      <c r="S3" s="13"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="S3" s="14"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="13" t="s">
+      <c r="V3" s="13"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="V3" s="14"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="13" t="s">
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="13" t="s">
+      <c r="S4" s="13"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="S4" s="14"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="13" t="s">
+      <c r="V4" s="13"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="V4" s="14"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="14"/>
-      <c r="W5" s="15"/>
+        <v>29</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="14"/>
       <c r="X5" s="8"/>
     </row>
     <row r="6" spans="1:24" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="13" t="s">
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="13" t="s">
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="13" t="s">
+      <c r="S6" s="13"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="S6" s="14"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="24" t="s">
+      <c r="V6" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="V6" s="24" t="s">
+      <c r="W6" s="16" t="s">
         <v>37</v>
-      </c>
-      <c r="W6" s="24" t="s">
-        <v>38</v>
       </c>
       <c r="X6" s="9"/>
     </row>
     <row r="7" spans="1:24" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="13" t="s">
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="13" t="s">
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="24" t="s">
+      <c r="S7" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="S7" s="26" t="s">
+      <c r="T7" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="T7" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="U7" s="25"/>
-      <c r="V7" s="25"/>
-      <c r="W7" s="25"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
       <c r="X7" s="9"/>
     </row>
     <row r="8" spans="1:24" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="C8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="13" t="s">
+      <c r="F8" s="14"/>
+      <c r="G8" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="9" t="s">
+      <c r="H8" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="I8" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="J8" s="14"/>
+      <c r="K8" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="J8" s="15"/>
-      <c r="K8" s="23" t="s">
+      <c r="L8" s="14"/>
+      <c r="M8" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="L8" s="15"/>
-      <c r="M8" s="9" t="s">
+      <c r="N8" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="N8" s="9" t="s">
+      <c r="O8" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="O8" s="10" t="s">
+      <c r="P8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="P8" s="11" t="s">
+      <c r="Q8" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="Q8" s="9" t="s">
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="V8" s="14"/>
-      <c r="W8" s="15"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="14"/>
       <c r="X8" s="9"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3027,19 +2410,18 @@
     <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="U8:W8"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="V6:V7"/>
-    <mergeCell ref="W6:W7"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="U4:W4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="J3:K4"/>
+    <mergeCell ref="L3:M4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="N4:Q4"/>
     <mergeCell ref="U3:W3"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="R1:T1"/>
@@ -3056,146 +2438,25 @@
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="H2:M2"/>
     <mergeCell ref="H3:I4"/>
-    <mergeCell ref="J3:K4"/>
-    <mergeCell ref="L3:M4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="H6:M6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="T7:T8"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="H7:M7"/>
     <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="U4:W4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="H5:M5"/>
-    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="U8:W8"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="W6:W7"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="R6:T6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C100"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="57.109375" customWidth="1"/>
-    <col min="2" max="2" width="76.44140625" customWidth="1"/>
-    <col min="3" max="3" width="44.21875" customWidth="1"/>
-    <col min="4" max="11" width="8.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-</worksheet>
 </file>
</xml_diff>